<commit_message>
update Pyrchase Requisition Xpath
</commit_message>
<xml_diff>
--- a/provide/test/TestDataProvideSBS.xlsx
+++ b/provide/test/TestDataProvideSBS.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -179,9 +179,6 @@
     <t>STANDARD</t>
   </si>
   <si>
-    <t>EMEAAD\proch</t>
-  </si>
-  <si>
     <t>Approver3</t>
   </si>
   <si>
@@ -212,15 +209,9 @@
     <t>10</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>300</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Aix  Golf</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Purchase requisition</t>
   </si>
   <si>
-    <t>146</t>
-  </si>
-  <si>
     <t>136</t>
   </si>
   <si>
@@ -248,39 +236,15 @@
     <t>TEST_AUTO_OAR_08032022_01</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_02</t>
-  </si>
-  <si>
     <t>TEST_AUTO_OAR_08032022_03</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_04</t>
-  </si>
-  <si>
-    <t>Product2</t>
-  </si>
-  <si>
     <t>Product3</t>
   </si>
   <si>
-    <t>Product4</t>
-  </si>
-  <si>
-    <t>LOGISTICS</t>
-  </si>
-  <si>
-    <t>BUILDINGS MAINTENANCE</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Logistic</t>
-  </si>
-  <si>
-    <t>CP-AAST</t>
-  </si>
-  <si>
     <t>4290</t>
   </si>
   <si>
@@ -290,27 +254,9 @@
     <t>S00007077001</t>
   </si>
   <si>
-    <t>S00010321001</t>
-  </si>
-  <si>
     <t>Contractors</t>
   </si>
   <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>Auditor fees</t>
-  </si>
-  <si>
-    <t>S00010242001</t>
-  </si>
-  <si>
-    <t>4293</t>
-  </si>
-  <si>
-    <t>EMEAAD\dcoisplet</t>
-  </si>
-  <si>
     <t>190000</t>
   </si>
   <si>
@@ -318,12 +264,6 @@
   </si>
   <si>
     <t>EMEAAD\pbuisson</t>
-  </si>
-  <si>
-    <t>185000</t>
-  </si>
-  <si>
-    <t>EMEAAD\laroche</t>
   </si>
 </sst>
 </file>
@@ -718,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>33</v>
@@ -850,7 +790,7 @@
         <v>27</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,10 +807,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>26</v>
@@ -879,25 +819,25 @@
         <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>37</v>
@@ -906,49 +846,49 @@
         <v>36</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="AF2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -965,282 +905,86 @@
         <v>21</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1248,14 +992,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>